<commit_message>
Updating trends analyze to use new bootstrapping
</commit_message>
<xml_diff>
--- a/replication/temp/figureA1_police_report_only.xlsx
+++ b/replication/temp/figureA1_police_report_only.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -34,70 +34,64 @@
     <t>total_dof</t>
   </si>
   <si>
-    <t>(8.64)</t>
-  </si>
-  <si>
-    <t>(4.87)</t>
-  </si>
-  <si>
-    <t>(1.31)</t>
-  </si>
-  <si>
-    <t>(1.08)</t>
-  </si>
-  <si>
-    <t>(0.5)</t>
-  </si>
-  <si>
-    <t>(0.37)</t>
-  </si>
-  <si>
-    <t>(1.92)</t>
-  </si>
-  <si>
-    <t>(1.63)</t>
-  </si>
-  <si>
-    <t>(0.96)</t>
-  </si>
-  <si>
-    <t>(0.28)</t>
-  </si>
-  <si>
-    <t>(1.41)</t>
+    <t>(2.57)</t>
+  </si>
+  <si>
+    <t>(1.96)</t>
+  </si>
+  <si>
+    <t>(0.62)</t>
+  </si>
+  <si>
+    <t>(0.1)</t>
+  </si>
+  <si>
+    <t>(0.57)</t>
   </si>
   <si>
     <t>(0.56)</t>
   </si>
   <si>
-    <t>(3.23)</t>
+    <t>(2.71)</t>
+  </si>
+  <si>
+    <t>(1.46)</t>
+  </si>
+  <si>
+    <t>(0.27)</t>
+  </si>
+  <si>
+    <t>(0.55)</t>
+  </si>
+  <si>
+    <t>(0.09)</t>
+  </si>
+  <si>
+    <t>(0.47)</t>
+  </si>
+  <si>
+    <t>(0.36)</t>
   </si>
   <si>
     <t>(2.09)</t>
   </si>
   <si>
-    <t>(2.16)</t>
-  </si>
-  <si>
-    <t>(3.99)</t>
-  </si>
-  <si>
-    <t>(0.22)</t>
-  </si>
-  <si>
-    <t>(0.29)</t>
-  </si>
-  <si>
-    <t>(4.27)</t>
-  </si>
-  <si>
-    <t>(3.64)</t>
-  </si>
-  <si>
-    <t>(3.48)</t>
-  </si>
-  <si>
-    <t>(3.43)</t>
+    <t>(1.45)</t>
+  </si>
+  <si>
+    <t>(0.7)</t>
+  </si>
+  <si>
+    <t>(0.8)</t>
+  </si>
+  <si>
+    <t>(2.0)</t>
+  </si>
+  <si>
+    <t>(0.51)</t>
+  </si>
+  <si>
+    <t>(1.56)</t>
   </si>
 </sst>
 </file>
@@ -592,22 +586,22 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s">
         <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -668,22 +662,22 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
         <v>25</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12">

</xml_diff>